<commit_message>
day 20 (121019) Apache POI reading data from excel file for DDT
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashley/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/IntelliJ IDEA CE.app/Summer2019OnlineTestNGSeleniumProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA4E5917-ED45-5E48-BE02-A3AAB2766DDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67DEFD-D589-0743-8E94-44016A71B30A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14780" xr2:uid="{205C05E0-4C92-0E43-BEF4-1DB18C9978F2}"/>
   </bookViews>
@@ -30,22 +30,22 @@
     <t>License Plate</t>
   </si>
   <si>
-    <t>test_plates_123</t>
-  </si>
-  <si>
     <t>Driver</t>
   </si>
   <si>
-    <t>Michael Schumacher</t>
-  </si>
-  <si>
     <t>Model Year</t>
   </si>
   <si>
     <t>Color</t>
   </si>
   <si>
-    <t>red</t>
+    <t>Fernando Alonso</t>
+  </si>
+  <si>
+    <t>TEST-PLATE</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,24 +424,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>2020</v>
+        <v>2001</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>

</xml_diff>